<commit_message>
finalized graphs for presentation
</commit_message>
<xml_diff>
--- a/Table_1.xlsx
+++ b/Table_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelly\Documents\Belize-MP-Bruno-Boos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4497669E-054B-4FE8-80AF-FBE646BCDAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D8AC38-DC4F-40EB-B4FE-CD23DFF3F4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{500167FE-CAAE-4500-BA2E-F6F75D4D8AFE}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="11700" windowHeight="11370" xr2:uid="{500167FE-CAAE-4500-BA2E-F6F75D4D8AFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="132">
   <si>
     <t>Common Name</t>
   </si>
@@ -56,12 +56,6 @@
     <t>Order</t>
   </si>
   <si>
-    <t>Number of Detections</t>
-  </si>
-  <si>
-    <t>Occupancy (95% BCI)</t>
-  </si>
-  <si>
     <t>Agouti</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t xml:space="preserve">Stable </t>
   </si>
   <si>
-    <t>Baird's Tapir</t>
-  </si>
-  <si>
     <t>Tapirus bairdii</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>Perissodactyla</t>
   </si>
   <si>
-    <t>Crested Guan</t>
-  </si>
-  <si>
     <t>Penelope purpurascens</t>
   </si>
   <si>
@@ -128,42 +116,27 @@
     <t>Carnivora</t>
   </si>
   <si>
-    <t>Great curassow</t>
-  </si>
-  <si>
     <t>Crax rubra</t>
   </si>
   <si>
     <t>VU</t>
   </si>
   <si>
-    <t>Jaguar</t>
-  </si>
-  <si>
     <t>Panthera onca</t>
   </si>
   <si>
     <t>Felidae</t>
   </si>
   <si>
-    <t xml:space="preserve">Ocellated turkey </t>
-  </si>
-  <si>
     <t>Meleagris ocellata</t>
   </si>
   <si>
     <t>Phasianidae</t>
   </si>
   <si>
-    <t xml:space="preserve">Ocelot </t>
-  </si>
-  <si>
     <t>Leopardus pardalis</t>
   </si>
   <si>
-    <t>Paca (same as agouti possibly)</t>
-  </si>
-  <si>
     <t>Cuniculus paca</t>
   </si>
   <si>
@@ -173,15 +146,9 @@
     <t>Rodentia</t>
   </si>
   <si>
-    <t>Puma</t>
-  </si>
-  <si>
     <t>Puma concolor</t>
   </si>
   <si>
-    <t>Red brocket</t>
-  </si>
-  <si>
     <t>Mazama americana</t>
   </si>
   <si>
@@ -221,9 +188,6 @@
     <t>Didelphimorphia</t>
   </si>
   <si>
-    <t>Great Tinamou</t>
-  </si>
-  <si>
     <t>Tinamus major</t>
   </si>
   <si>
@@ -233,24 +197,12 @@
     <t>Tinamiformes</t>
   </si>
   <si>
-    <t>Ruddy Quail-dove</t>
-  </si>
-  <si>
     <t>Geotrygon montana</t>
   </si>
   <si>
-    <t>Margay</t>
-  </si>
-  <si>
     <t>Leopardus wiedii</t>
   </si>
   <si>
-    <t>Central American Tapir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">same as bairds </t>
-  </si>
-  <si>
     <t>Tayra</t>
   </si>
   <si>
@@ -260,9 +212,6 @@
     <t>Mustelidae</t>
   </si>
   <si>
-    <t>Striped Hog-nosed Skunk</t>
-  </si>
-  <si>
     <t>Conepatus semistriatus</t>
   </si>
   <si>
@@ -272,9 +221,6 @@
     <t>Mephitidae</t>
   </si>
   <si>
-    <t>Bare-throated Tiger Heron</t>
-  </si>
-  <si>
     <t>Tigrisoma mexicanum</t>
   </si>
   <si>
@@ -284,27 +230,18 @@
     <t>Pelecaniformes</t>
   </si>
   <si>
-    <t>Collared Peccary</t>
-  </si>
-  <si>
     <t>Dicotyles tajacu</t>
   </si>
   <si>
     <t>Tayassuidae (formally Suidae)</t>
   </si>
   <si>
-    <t>White-lipped Peccary</t>
-  </si>
-  <si>
     <t>Tayassu pecari</t>
   </si>
   <si>
     <t>Tayassuidae</t>
   </si>
   <si>
-    <t>Wood Thrush</t>
-  </si>
-  <si>
     <t>Hylocichla mustelina</t>
   </si>
   <si>
@@ -314,9 +251,6 @@
     <t>Passeriformes</t>
   </si>
   <si>
-    <t>Russet-naped Wood Rail</t>
-  </si>
-  <si>
     <t>Aramides albiventris</t>
   </si>
   <si>
@@ -326,9 +260,6 @@
     <t>Aramides</t>
   </si>
   <si>
-    <t>Nine-banded Armadillo</t>
-  </si>
-  <si>
     <t>Dasypus novemcinctus</t>
   </si>
   <si>
@@ -338,20 +269,176 @@
     <t>Cingulata</t>
   </si>
   <si>
-    <t xml:space="preserve">Brown Four-eyed Oppossum </t>
-  </si>
-  <si>
     <t>Metachirus nudicaudatus</t>
   </si>
   <si>
     <t>Dasyproctidae</t>
+  </si>
+  <si>
+    <t>Mean Predicted Occupancy</t>
+  </si>
+  <si>
+    <t>SE Predicted Occupancy</t>
+  </si>
+  <si>
+    <t>0.32 </t>
+  </si>
+  <si>
+    <t>0.009 </t>
+  </si>
+  <si>
+    <t>0.69 </t>
+  </si>
+  <si>
+    <t>0.01 </t>
+  </si>
+  <si>
+    <t>0.25 </t>
+  </si>
+  <si>
+    <t>0.007 </t>
+  </si>
+  <si>
+    <t>0.48 </t>
+  </si>
+  <si>
+    <t>0.67 </t>
+  </si>
+  <si>
+    <t>0.012 </t>
+  </si>
+  <si>
+    <t>0.52 </t>
+  </si>
+  <si>
+    <t>0.013 </t>
+  </si>
+  <si>
+    <t>0.70 </t>
+  </si>
+  <si>
+    <t>0.011 </t>
+  </si>
+  <si>
+    <t>0.71 </t>
+  </si>
+  <si>
+    <t>0.73 </t>
+  </si>
+  <si>
+    <t>0.006 </t>
+  </si>
+  <si>
+    <t>0.20 </t>
+  </si>
+  <si>
+    <t>0.44 </t>
+  </si>
+  <si>
+    <t>0.29 </t>
+  </si>
+  <si>
+    <t>0.11 </t>
+  </si>
+  <si>
+    <t>0.005 </t>
+  </si>
+  <si>
+    <t>0.34 </t>
+  </si>
+  <si>
+    <t>0.80  </t>
+  </si>
+  <si>
+    <t>0.008 </t>
+  </si>
+  <si>
+    <t>0.03 </t>
+  </si>
+  <si>
+    <t>0.002 </t>
+  </si>
+  <si>
+    <t>0.37 </t>
+  </si>
+  <si>
+    <t>0.51 </t>
+  </si>
+  <si>
+    <t>0.015 </t>
+  </si>
+  <si>
+    <t>Russet-naped wood Rail</t>
+  </si>
+  <si>
+    <t>White-lipped peccary</t>
+  </si>
+  <si>
+    <t>Collared peccary</t>
+  </si>
+  <si>
+    <t>Striped hog-nosed skunk</t>
+  </si>
+  <si>
+    <t>Nine-banded armadillo</t>
+  </si>
+  <si>
+    <t>Ruddy quail-dove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brown four-eyed oppossum </t>
+  </si>
+  <si>
+    <t>Crested guan</t>
+  </si>
+  <si>
+    <t>Wood thrush</t>
+  </si>
+  <si>
+    <t>Bare-throated tiger heron</t>
+  </si>
+  <si>
+    <t>Paca</t>
+  </si>
+  <si>
+    <t>Great tinamou</t>
+  </si>
+  <si>
+    <t>Dasyprocta punctata </t>
+  </si>
+  <si>
+    <t>No. of Detections</t>
+  </si>
+  <si>
+    <t>Baird's tapir*</t>
+  </si>
+  <si>
+    <t>Puma*</t>
+  </si>
+  <si>
+    <t>Jaguar*</t>
+  </si>
+  <si>
+    <t>Ocellated turkey*</t>
+  </si>
+  <si>
+    <t>Red brocket*</t>
+  </si>
+  <si>
+    <t>Ocelot*</t>
+  </si>
+  <si>
+    <t>Margay*</t>
+  </si>
+  <si>
+    <t>Great curassow*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,25 +459,32 @@
       <name val="Palatino Linotype"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -405,12 +499,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,21 +824,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3924DA67-0EA0-40C8-B42D-5CAB72CC6F71}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -752,680 +851,774 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+        <v>79</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>93</v>
+        <v>110</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="G2" s="2">
         <v>49</v>
       </c>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="K2" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>128</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G3" s="2">
         <v>493</v>
       </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G4" s="2">
         <v>1836</v>
       </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>86</v>
+        <v>111</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G5" s="2">
         <v>65</v>
       </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>83</v>
+        <v>112</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G6" s="2">
         <v>73</v>
       </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G7" s="2">
         <v>2475</v>
       </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>126</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G8" s="2">
         <v>288</v>
       </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>129</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G9" s="2">
         <v>781</v>
       </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>125</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G10" s="2">
         <v>554</v>
       </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>68</v>
+        <v>130</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G11" s="2">
         <v>101</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" t="s">
+        <v>96</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>75</v>
+        <v>113</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G12" s="2">
         <v>86</v>
       </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>72</v>
+        <v>55</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G13" s="2">
         <v>95</v>
       </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G14" s="2">
         <v>318</v>
       </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" t="s">
+        <v>93</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>97</v>
+        <v>114</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="G15" s="2">
         <v>42</v>
       </c>
       <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="K15" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G16" s="2">
         <v>443</v>
       </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>66</v>
+        <v>115</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G17" s="2">
         <v>107</v>
       </c>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" t="s">
+        <v>101</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="G18" s="2">
         <v>206</v>
       </c>
       <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="K18" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>101</v>
+        <v>116</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="G19" s="2">
         <v>41</v>
       </c>
       <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="K19" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G20" s="2">
         <v>213</v>
       </c>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H20" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I20" t="s">
+        <v>93</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>131</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G21" s="2">
         <v>2737</v>
       </c>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I21" t="s">
+        <v>104</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>37</v>
+        <v>127</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G22" s="2">
         <v>2878</v>
       </c>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I22" t="s">
+        <v>93</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>89</v>
+        <v>118</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>90</v>
+        <v>11</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="G23" s="2">
         <v>60</v>
       </c>
       <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="K23" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>79</v>
+        <v>119</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G24" s="2">
         <v>82</v>
       </c>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I24" t="s">
+        <v>106</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="2">
+        <v>403</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="K25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="2">
-        <v>304</v>
-      </c>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="26" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>120</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="G26" s="2">
         <v>468</v>
       </c>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
-      <c r="A27" s="4" t="s">
+      <c r="H26" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" t="s">
+        <v>91</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="A27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="G27" s="2">
         <v>877</v>
       </c>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="H27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I27" t="s">
+        <v>109</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>62</v>
+        <v>121</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G28" s="2">
         <v>109</v>
       </c>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.5" x14ac:dyDescent="0.4">
-      <c r="A29" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2">
-        <v>99</v>
-      </c>
-      <c r="H29" s="2"/>
+      <c r="H28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I28" t="s">
+        <v>104</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H29">

</xml_diff>